<commit_message>
Website developments - shipping address, review order
</commit_message>
<xml_diff>
--- a/Docs/WarrierCards-Tasks.xlsx
+++ b/Docs/WarrierCards-Tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
   <si>
     <t>No</t>
   </si>
@@ -213,13 +213,22 @@
   </si>
   <si>
     <t>Sell with us</t>
+  </si>
+  <si>
+    <t>Payment gateway integration</t>
+  </si>
+  <si>
+    <t>Card customization</t>
+  </si>
+  <si>
+    <t>If user input slash in keyword textbox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +240,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,10 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,7 +838,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -1062,12 +1079,27 @@
         <v>63</v>
       </c>
     </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>48</v>
       </c>
       <c r="D26" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>